<commit_message>
created test data for the knowledge sharing session
</commit_message>
<xml_diff>
--- a/reports/test_login_report.xlsx
+++ b/reports/test_login_report.xlsx
@@ -1141,12 +1141,12 @@
       </c>
       <c r="H14" s="3" t="inlineStr">
         <is>
-          <t>Login functionality verified</t>
-        </is>
-      </c>
-      <c r="I14" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>Verify visibility of 'don't have an account' text on login page.</t>
+          <t>Verify visibility of "Don't have an account?" text on login page.</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">

</xml_diff>